<commit_message>
programme updated + press
</commit_message>
<xml_diff>
--- a/content/temp_Rooms_Hyperion.xlsx
+++ b/content/temp_Rooms_Hyperion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/other/semantics.github.io/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816563C3-7F0B-A743-A645-773CED9D3422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3815563E-CAAA-A644-AB11-DEF2C374FCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="27460" windowHeight="16520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="27460" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="104">
   <si>
     <t>9:00 - 10:00</t>
   </si>
@@ -66,10 +66,6 @@
     <t>Group: Dbpedia
 Slot title: DBpedia
 Title: DBpedia Keynote</t>
-  </si>
-  <si>
-    <t>Group: Tutorial
-Slot title: Tutorial</t>
   </si>
   <si>
     <t>Group: Break
@@ -971,12 +967,425 @@
 Author: Ilan Kernermann (Lexicala) &amp; Martin Kaltenböck (SemanticWeb Company)
 Title: Fostering Data Spaces interoperability with Language Models and Knowledge Graphs</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tutorial
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Key to Sustainable Enterprises: ESG, Knowledge Graphs, and Digitalization</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tutorial
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Streamlining License Customization and Clearance with Open DALICC Framework</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tutorial
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Open Research Knowledge Graph</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tutorial
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modular Approach to Solve Problems at Scale with Healthcare NLP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Beginners' Guide to Reasoning</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Knowledge Engineering of Taxonomies and Ontologies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Group: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Slot title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tutorial
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Beginners' Guide to Reasoning</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1031,6 +1440,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1049,12 +1473,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEA9999"/>
-        <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
     <fill>
@@ -1081,6 +1499,12 @@
         <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1139,19 +1563,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1171,11 +1592,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1397,8 +1821,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1412,22 +1836,22 @@
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1438,111 +1862,113 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>91</v>
+      <c r="G6" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="8" t="s">
+      <c r="B8" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="1"/>
@@ -1551,46 +1977,48 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1"/>
+      <c r="B10" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>100</v>
+      </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="9" t="s">
-        <v>87</v>
+      <c r="G10" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="B11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1618,353 +2046,353 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="14"/>
+    <col min="1" max="1" width="12.6640625" style="13"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="18"/>
+      <c r="F2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>25</v>
+      <c r="A3" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="18"/>
+      <c r="F3" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" ht="14" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-    </row>
-    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="B9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="G11" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="B13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="G14" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="B15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="B16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="G16" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="B17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="B18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1987,7 +2415,7 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1996,22 +2424,22 @@
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.2">
@@ -2022,296 +2450,296 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="18"/>
+      <c r="F2" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="272" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="22"/>
+        <v>60</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:9" ht="221" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="22"/>
+        <v>61</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:9" ht="238" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="356" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="289" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="22"/>
+        <v>82</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+        <v>55</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:9" ht="231" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="I16" s="15"/>
+      <c r="F16" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="G17" s="18"/>
+      <c r="G17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>